<commit_message>
Update Manual Tests for 4.2 Release
</commit_message>
<xml_diff>
--- a/Project-Management/Tools/RoadmapUpdate/issue_template.xlsx
+++ b/Project-Management/Tools/RoadmapUpdate/issue_template.xlsx
@@ -5,22 +5,25 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mantid\Documents\Project-Management\Tools\RoadmapUpdate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\documents\Project-Management\Tools\RoadmapUpdate\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="34545" yWindow="-12855" windowWidth="31665" windowHeight="16500"/>
+    <workbookView xWindow="34545" yWindow="-12855" windowWidth="31665" windowHeight="16500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="issues" sheetId="1" r:id="rId1"/>
     <sheet name="assignees" sheetId="2" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="142">
   <si>
     <t>Title</t>
   </si>
@@ -239,15 +242,6 @@
   </si>
   <si>
     <t>Unscripted Testing ISIS Reflectometry (old and new)</t>
-  </si>
-  <si>
-    <t>Unscripted Testing ISIS SANS (v2 GUI)</t>
-  </si>
-  <si>
-    <t>Unsrtipted testing M-slice</t>
-  </si>
-  <si>
-    <t>Unscripted Testing - Mantid Basics Course</t>
   </si>
   <si>
     <t>ElliotAOram</t>
@@ -270,13 +264,7 @@
 * workflow diagrams should appear on algorithm pages in offline help</t>
   </si>
   <si>
-    <t>Unscripted testing - project recovery</t>
-  </si>
-  <si>
     <t>http://developer.mantidproject.org/Testing/ErrorReporter-ProjectRecovery/ProjectRecoveryTesting.html</t>
-  </si>
-  <si>
-    <t>Unscripted testing - error reporter</t>
   </si>
   <si>
     <t>http://developer.mantidproject.org/Testing/ErrorReporter-ProjectRecovery/ErrorReporterTesting.html</t>
@@ -358,84 +346,6 @@
   </si>
   <si>
     <t>Rob Applin</t>
-  </si>
-  <si>
-    <t># SANS GUI Testing
-&lt;div class="contents" data-local=""&gt;
-&lt;/div&gt;
-## Data reduction
-*Preparation*
-  - Get the ISIS sample data from the website
-  - Ensure that the ISIS sample data directory is in the search
-    directories
-**Time required 20 - 30 minutes**
------
-1.  Open `Interfaces` \&gt; `SANS` \&gt; `SANS v2`
-2.  Set `Instrument` to `LOQ`
-3.  Choose `Load User File`; from the ISIS sample data in the `loqdemo`
-    folder, choose `Maskfile.txt`
-4.  Choose `Load Batch File`; from the ISIS sample data in the
-    &lt;span class="title-ref"&gt;loqdemo&lt;/span&gt; folder, choose
-    `batch_mode_reduction.csv`
-5.    - In the `Settings` tab:
-          - Go to `Mask`
-          - Click `Display Mask`
-          - This should give an instrument view with a circle at the
-            centre
-6.    - In the `Runs` tab
-          - Click `Process`
-          - After some seconds the rows should turn green
-          - In the Main window there should be a series of new
-            workspaces; 3 group workspaces and 4 2D workspaces
-          - Change the first column of the first row to 74045; click
-            process
-          - The row should turn blue; hovering over the row should give
-            an error message
-          - Change the `Reduction` button to 2D
-          - Check the `Plot Results` box
-          - Click `Process`
-          - A plot window will open; initially empty, then with a red
-            line
-          - Change `Reduction` back to 1D
-          - Click `Process`
-          - In the plot you should end up with a red and a black line
-            plotted
-          - Check the `Multi-period` box
-          - 6 additional rows should appear in the table
-          - Check that the `Add`, `Delete`, `Copy`, `Paste`, `Cut` and
-            `Erase` icons work as expected
-          - Delete all rows and re-load the batch file as previously
-7.    - In the `Settings` tab
-          - Set `Reduction Type` to `Merged`
-          - Return to the `Runs` tab
-          - Ensure `Plot results` is checked
-          - Click `Process`
-          - This should result in a plot with three lines
-8.    - In the `Beam centre` tab
-          - Click
-          - A plot should appear after some seconds, with 4 lines
-          - The 4 lines should gradually get closer together
-          - This will run for some time, probably minutes
-9.    - In the `Sum Runs` tab
-          - Enter `74044, 74019` in the top line
-          - Enter `LOQ74044-add` as Output file
-          - Ensure that the `Output directory` is in you r managed paths
-          - Click `Sum` at the bottom
-          - Go back to the `Runs` tab
-          - Remove all rows
-          - Reload the batch file as before
-          - Change the first column of both rows to `LOQ74044-add`
-          - Click `Process`
-          - This should now process as before
-10.   - In the `Diagnostic Page` tab
-          - For run choose `Browse` and load the `LOQ74044.nxs` file
-          - Click each of the `Integral` buttons
-          - They should produce plots
-          - Check the `Apply Mask` boxes and click the buttons again
-          - They should produce new, slightly different plots
-11.   - In the `Runs` tab
-          - Check all variables and inputs for tool tips by hovering
-            over them</t>
   </si>
   <si>
     <t># VSI Testing
@@ -515,10 +425,6 @@
     <t>?</t>
   </si>
   <si>
-    <t xml:space="preserve">
-See https://www.mantidproject.org/MBC_Live_Data_Simple_Examples</t>
-  </si>
-  <si>
     <t>alicerussell1</t>
   </si>
   <si>
@@ -568,13 +474,67 @@
   </si>
   <si>
     <t>See https://mantidproject.github.io/mslice/ and follow Quick Start, this should probably be tested in iDAaaS</t>
+  </si>
+  <si>
+    <t>DanielMurphy22</t>
+  </si>
+  <si>
+    <t>DannyHindson</t>
+  </si>
+  <si>
+    <t>RichardWaiteSTFC</t>
+  </si>
+  <si>
+    <t>StephenSmith25</t>
+  </si>
+  <si>
+    <t>DavidFair</t>
+  </si>
+  <si>
+    <t>David Fair</t>
+  </si>
+  <si>
+    <t>Unscripted testing Project Recovery</t>
+  </si>
+  <si>
+    <t>Unscripted testing Error Reporter</t>
+  </si>
+  <si>
+    <t>Unscripted Testing  Mantid Basics Course</t>
+  </si>
+  <si>
+    <t>Unscripted Testing M-slice</t>
+  </si>
+  <si>
+    <t>Stephen Smith</t>
+  </si>
+  <si>
+    <t>Daniel Murphy</t>
+  </si>
+  <si>
+    <t>Richard Waite</t>
+  </si>
+  <si>
+    <t>Danny Hindson</t>
+  </si>
+  <si>
+    <t>Unscripted Testing ISIS SANS (new GUI)</t>
+  </si>
+  <si>
+    <t>See https://developer.mantidproject.org/Testing/SANSGUI/SANSGUITests.html</t>
+  </si>
+  <si>
+    <t>See https://developer.mantidproject.org/Testing/LiveData/LiveDataTests.html</t>
+  </si>
+  <si>
+    <t>Link made in mantid PR #27128</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="22">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -717,11 +677,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF666666"/>
-      <name val="Cambria (Headings)"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1079,7 +1034,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1092,11 +1047,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1154,6 +1112,19 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="assignees"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1443,13 +1414,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G32" sqref="G30:G32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="46" style="1" customWidth="1"/>
     <col min="2" max="2" width="72.7109375" style="1" customWidth="1"/>
@@ -1457,7 +1428,7 @@
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1468,93 +1439,93 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="60">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>117</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="105">
+    <row r="5" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>104</v>
+        <v>77</v>
+      </c>
+      <c r="C5" t="s">
+        <v>119</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="60">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>81</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>120</v>
+        <v>75</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>124</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="16.5">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>116</v>
+        <v>75</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>125</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -1562,14 +1533,14 @@
         <f>B8</f>
         <v>See https://www.mantidproject.org/Unscripted_Manual_Testing#Groups</v>
       </c>
-      <c r="C9" t="s">
-        <v>128</v>
+      <c r="C9" s="7" t="s">
+        <v>126</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.75">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1577,14 +1548,14 @@
         <f>B9</f>
         <v>See https://www.mantidproject.org/Unscripted_Manual_Testing#Groups</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>124</v>
+      <c r="C10" s="1" t="s">
+        <v>127</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -1592,284 +1563,287 @@
         <f>B10</f>
         <v>See https://www.mantidproject.org/Unscripted_Manual_Testing#Groups</v>
       </c>
-      <c r="C11" t="s">
-        <v>122</v>
+      <c r="C11" s="6" t="s">
+        <v>113</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="75">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C12" t="s">
-        <v>126</v>
+        <v>80</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="45">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>51</v>
+        <v>94</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>107</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C14" t="s">
-        <v>70</v>
+        <v>35</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="12.75" customHeight="1">
+    <row r="16" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="8" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="8" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="409.5">
+    <row r="21" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>34</v>
+        <v>119</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="60">
+    <row r="24" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C24" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="75.75">
+    <row r="26" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>116</v>
+        <v>51</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="30">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>102</v>
+      <c r="C27" t="s">
+        <v>115</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="409.5">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>73</v>
+        <v>138</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>108</v>
+        <v>139</v>
       </c>
       <c r="C28" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="30">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>113</v>
+        <v>140</v>
       </c>
       <c r="C29" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="105">
+        <v>105</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>75</v>
+        <v>132</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C30" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C31" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="30">
-      <c r="A31" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="30">
-      <c r="A32" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="30">
+    </row>
+    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>83</v>
+        <v>131</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:F7"/>
   </dataValidations>
   <hyperlinks>
@@ -1879,30 +1853,18 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>assignees!$A$2:$A$181</xm:f>
+            <xm:f>[issue_templateupdate.xlsx]assignees!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>C7</xm:sqref>
+          <xm:sqref>C34:C40</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>assignees!$A$2:$A$181</xm:f>
+            <xm:f>assignees!$A$2:$A$37</xm:f>
           </x14:formula1>
-          <xm:sqref>C12:C18</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>assignees!$A$2:$A$181</xm:f>
-          </x14:formula1>
-          <xm:sqref>C20:C26 C28:C40 C5</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>assignees!$A$2:$A$181</xm:f>
-          </x14:formula1>
-          <xm:sqref>C27 C3:C4</xm:sqref>
+          <xm:sqref>C2:C33</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1912,19 +1874,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32:C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>69</v>
       </c>
@@ -1932,10 +1894,10 @@
         <v>30</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -1947,7 +1909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -1956,10 +1918,10 @@
       </c>
       <c r="C3">
         <f>COUNTIF(issues!$C:$C,assignees!A3)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -1968,10 +1930,10 @@
       </c>
       <c r="C4">
         <f>COUNTIF(issues!$C:$C,assignees!A4)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -1983,7 +1945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -1995,7 +1957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -2007,7 +1969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -2019,19 +1981,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B9" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C9">
         <f>COUNTIF(issues!$C:$C,assignees!A9)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -2043,7 +2005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>47</v>
       </c>
@@ -2052,10 +2014,10 @@
       </c>
       <c r="C11">
         <f>COUNTIF(issues!$C:$C,assignees!A11)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -2067,7 +2029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>49</v>
       </c>
@@ -2079,7 +2041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>55</v>
       </c>
@@ -2091,7 +2053,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>70</v>
       </c>
@@ -2100,46 +2062,46 @@
       </c>
       <c r="C15">
         <f>COUNTIF(issues!$C:$C,assignees!A15)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B16" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C16">
         <f>COUNTIF(issues!$C:$C,assignees!A16)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B17" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C17">
         <f>COUNTIF(issues!$C:$C,assignees!A17)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B18" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C18">
         <f>COUNTIF(issues!$C:$C,assignees!A18)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>61</v>
       </c>
@@ -2151,7 +2113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>65</v>
       </c>
@@ -2163,19 +2125,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B21" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C21">
         <f>COUNTIF(issues!$C:$C,assignees!A21)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -2187,7 +2149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>57</v>
       </c>
@@ -2199,7 +2161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>59</v>
       </c>
@@ -2211,7 +2173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>63</v>
       </c>
@@ -2223,7 +2185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>67</v>
       </c>
@@ -2235,75 +2197,135 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B27" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C27">
         <f>COUNTIF(issues!$C:$C,assignees!A27)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B28" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C28">
         <f>COUNTIF(issues!$C:$C,assignees!A28)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>121</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>114</v>
       </c>
       <c r="C29">
         <f>COUNTIF(issues!$C:$C,assignees!A29)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B30" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C30">
         <f>COUNTIF(issues!$C:$C,assignees!A30)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75">
-      <c r="A31" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>125</v>
+    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>118</v>
       </c>
       <c r="C31">
         <f>COUNTIF(issues!$C:$C,assignees!A31)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B32" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="C32">
         <f>COUNTIF(issues!$C:$C,assignees!A32)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>128</v>
+      </c>
+      <c r="B33" t="s">
+        <v>129</v>
+      </c>
+      <c r="C33">
+        <f>COUNTIF(issues!$C:$C,assignees!A33)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>127</v>
+      </c>
+      <c r="B34" t="s">
+        <v>134</v>
+      </c>
+      <c r="C34">
+        <f>COUNTIF(issues!$C:$C,assignees!A34)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>124</v>
+      </c>
+      <c r="B35" t="s">
+        <v>135</v>
+      </c>
+      <c r="C35">
+        <f>COUNTIF(issues!$C:$C,assignees!A35)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>126</v>
+      </c>
+      <c r="B36" t="s">
+        <v>136</v>
+      </c>
+      <c r="C36">
+        <f>COUNTIF(issues!$C:$C,assignees!A36)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>125</v>
+      </c>
+      <c r="B37" t="s">
+        <v>137</v>
+      </c>
+      <c r="C37">
+        <f>COUNTIF(issues!$C:$C,assignees!A37)</f>
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update location of unscripted testing
This commit updates the location of certain unscripted tests that had been moved from the regular mantid docs to the dev-docs
</commit_message>
<xml_diff>
--- a/Project-Management/Tools/RoadmapUpdate/issue_template.xlsx
+++ b/Project-Management/Tools/RoadmapUpdate/issue_template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\documents\Project-Management\Tools\RoadmapUpdate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wey38795\Documents\mantid_builds\documents\documents\Project-Management\Tools\RoadmapUpdate\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="34545" yWindow="-12855" windowWidth="31665" windowHeight="16500" activeTab="1"/>
+    <workbookView xWindow="34548" yWindow="-12852" windowWidth="31668" windowHeight="16500"/>
   </bookViews>
   <sheets>
     <sheet name="issues" sheetId="1" r:id="rId1"/>
@@ -270,10 +270,6 @@
     <t>http://developer.mantidproject.org/Testing/ErrorReporter-ProjectRecovery/ErrorReporterTesting.html</t>
   </si>
   <si>
-    <t>See instructions at http://docs.mantidproject.org/v3.9.0/interfaces/Muon_Analysis_unscripted_testing_guide.html
-http://developer.mantidproject.org/Testing/MuonInterface/MuonTesting.html</t>
-  </si>
-  <si>
     <t>Follow:  http://www.mantidproject.org/Direct:DgsReduction
      and http://www.mantidproject.org/Create_MD_Workspace_GUI#Direct_Inelastic_Mod_Q</t>
   </si>
@@ -303,9 +299,6 @@
   </si>
   <si>
     <t>small</t>
-  </si>
-  <si>
-    <t>Follow: http://docs.mantidproject.org/nightly/interfaces/Engineering%20Diffraction%20Test%20Guide.html</t>
   </si>
   <si>
     <t>* Follow the examples at http://docs.mantidproject.org/nightly/concepts/WorkspaceGroup.html 
@@ -528,6 +521,13 @@
   </si>
   <si>
     <t>Link made in mantid PR #27128</t>
+  </si>
+  <si>
+    <t>Follow: http://docs.mantidproject.org/nightly/Testing/Engineering%20Diffraction%20Test%20Guide.html</t>
+  </si>
+  <si>
+    <t>See instructions at http://docs.mantidproject.org/nightly/Testing/Muon_Analysis_unscripted_testing_guide.html
+http://developer.mantidproject.org/Testing/MuonInterface/MuonTesting.html</t>
   </si>
 </sst>
 </file>
@@ -1416,19 +1416,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G32" sqref="G30:G32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="46" style="1" customWidth="1"/>
-    <col min="2" max="2" width="72.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="72.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1439,24 +1439,24 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1464,7 +1464,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1472,7 +1472,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1480,38 +1480,38 @@
         <v>77</v>
       </c>
       <c r="C5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -1519,13 +1519,13 @@
         <v>75</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -1534,13 +1534,13 @@
         <v>See https://www.mantidproject.org/Unscripted_Manual_Testing#Groups</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1549,13 +1549,13 @@
         <v>See https://www.mantidproject.org/Unscripted_Manual_Testing#Groups</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -1564,55 +1564,55 @@
         <v>See https://www.mantidproject.org/Unscripted_Manual_Testing#Groups</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>80</v>
+        <v>141</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C14" t="s">
         <v>35</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -1620,7 +1620,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1628,7 +1628,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -1636,21 +1636,21 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -1658,7 +1658,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -1666,32 +1666,32 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>91</v>
+        <v>140</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -1702,21 +1702,21 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C24" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
@@ -1727,21 +1727,21 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>51</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>72</v>
       </c>
@@ -1749,88 +1749,88 @@
         <v>28</v>
       </c>
       <c r="C27" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C28" t="s">
         <v>47</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C29" t="s">
         <v>35</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C30" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="C31" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>78</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>79</v>
@@ -1839,7 +1839,7 @@
         <v>70</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1876,17 +1876,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C32" sqref="C32:C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>69</v>
       </c>
@@ -1894,10 +1894,10 @@
         <v>30</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -1909,7 +1909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -1921,7 +1921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -1945,7 +1945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -1957,7 +1957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -1969,7 +1969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -1981,19 +1981,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C9">
         <f>COUNTIF(issues!$C:$C,assignees!A9)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>47</v>
       </c>
@@ -2017,7 +2017,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -2029,7 +2029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>49</v>
       </c>
@@ -2041,7 +2041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>55</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>70</v>
       </c>
@@ -2065,43 +2065,43 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B16" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C16">
         <f>COUNTIF(issues!$C:$C,assignees!A16)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C17">
         <f>COUNTIF(issues!$C:$C,assignees!A17)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B18" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C18">
         <f>COUNTIF(issues!$C:$C,assignees!A18)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>61</v>
       </c>
@@ -2113,7 +2113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>65</v>
       </c>
@@ -2125,19 +2125,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B21" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C21">
         <f>COUNTIF(issues!$C:$C,assignees!A21)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -2149,7 +2149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>57</v>
       </c>
@@ -2161,7 +2161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>59</v>
       </c>
@@ -2173,7 +2173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>63</v>
       </c>
@@ -2185,7 +2185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>67</v>
       </c>
@@ -2197,7 +2197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>73</v>
       </c>
@@ -2209,120 +2209,120 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B28" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C28">
         <f>COUNTIF(issues!$C:$C,assignees!A28)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C29">
         <f>COUNTIF(issues!$C:$C,assignees!A29)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B30" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C30">
         <f>COUNTIF(issues!$C:$C,assignees!A30)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C31">
         <f>COUNTIF(issues!$C:$C,assignees!A31)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B32" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C32">
         <f>COUNTIF(issues!$C:$C,assignees!A32)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B33" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C33">
         <f>COUNTIF(issues!$C:$C,assignees!A33)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B34" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C34">
         <f>COUNTIF(issues!$C:$C,assignees!A34)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B35" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C35">
         <f>COUNTIF(issues!$C:$C,assignees!A35)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B36" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C36">
         <f>COUNTIF(issues!$C:$C,assignees!A36)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B37" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C37">
         <f>COUNTIF(issues!$C:$C,assignees!A37)</f>

</xml_diff>

<commit_message>
Update ISIS Reflectometry manual testing URL
</commit_message>
<xml_diff>
--- a/Project-Management/Tools/RoadmapUpdate/issue_template.xlsx
+++ b/Project-Management/Tools/RoadmapUpdate/issue_template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\documents\Project-Management\Tools\RoadmapUpdate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmo84564\mantid-documents\Project-Management\Tools\RoadmapUpdate\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="34545" yWindow="-12855" windowWidth="31665" windowHeight="16500" activeTab="1"/>
+    <workbookView xWindow="34545" yWindow="-12855" windowWidth="31665" windowHeight="16500"/>
   </bookViews>
   <sheets>
     <sheet name="issues" sheetId="1" r:id="rId1"/>
@@ -109,9 +109,6 @@
     <t>Unscripted Testing Sample Transmission calculator</t>
   </si>
   <si>
-    <t>For testing procedures see http://www.mantidproject.org/Testing_ISIS_Reflectometry_GUI</t>
-  </si>
-  <si>
     <t>Unscripted Testing Live Data ISIS</t>
   </si>
   <si>
@@ -239,9 +236,6 @@
   </si>
   <si>
     <t>Matthew Andrew</t>
-  </si>
-  <si>
-    <t>Unscripted Testing ISIS Reflectometry (old and new)</t>
   </si>
   <si>
     <t>ElliotAOram</t>
@@ -528,6 +522,12 @@
   </si>
   <si>
     <t>Link made in mantid PR #27128</t>
+  </si>
+  <si>
+    <t>Unscripted Testing ISIS Reflectometry</t>
+  </si>
+  <si>
+    <t>For testing procedures see http://developer.mantidproject.org/Testing/ReflectometryGUI/ReflectometryGUITests.html</t>
   </si>
 </sst>
 </file>
@@ -1416,8 +1416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G32" sqref="G30:G32"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A27" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1439,7 +1439,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1447,13 +1447,13 @@
         <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1461,7 +1461,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1469,7 +1469,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="105" x14ac:dyDescent="0.25">
@@ -1477,13 +1477,13 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1491,24 +1491,24 @@
         <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
@@ -1516,13 +1516,13 @@
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -1534,10 +1534,10 @@
         <v>See https://www.mantidproject.org/Unscripted_Manual_Testing#Groups</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1549,10 +1549,10 @@
         <v>See https://www.mantidproject.org/Unscripted_Manual_Testing#Groups</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1564,10 +1564,10 @@
         <v>See https://www.mantidproject.org/Unscripted_Manual_Testing#Groups</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -1575,27 +1575,27 @@
         <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1603,13 +1603,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1617,7 +1617,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1625,7 +1625,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1633,7 +1633,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1641,13 +1641,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1655,7 +1655,7 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1663,7 +1663,7 @@
         <v>19</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
@@ -1671,10 +1671,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1682,13 +1682,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1699,7 +1699,7 @@
         <v>23</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -1707,13 +1707,13 @@
         <v>24</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C24" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1724,7 +1724,7 @@
         <v>26</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -1732,114 +1732,114 @@
         <v>27</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>28</v>
+        <v>141</v>
       </c>
       <c r="C27" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C31" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1876,7 +1876,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C32" sqref="C32:C37"/>
     </sheetView>
   </sheetViews>
@@ -1888,21 +1888,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
         <v>32</v>
-      </c>
-      <c r="B2" t="s">
-        <v>33</v>
       </c>
       <c r="C2">
         <f>COUNTIF(issues!$C:$C,assignees!A2)</f>
@@ -1911,10 +1911,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3">
         <f>COUNTIF(issues!$C:$C,assignees!A3)</f>
@@ -1923,10 +1923,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s">
         <v>35</v>
-      </c>
-      <c r="B4" t="s">
-        <v>36</v>
       </c>
       <c r="C4">
         <f>COUNTIF(issues!$C:$C,assignees!A4)</f>
@@ -1935,10 +1935,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
         <v>37</v>
-      </c>
-      <c r="B5" t="s">
-        <v>38</v>
       </c>
       <c r="C5">
         <f>COUNTIF(issues!$C:$C,assignees!A5)</f>
@@ -1947,10 +1947,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s">
         <v>39</v>
-      </c>
-      <c r="B6" t="s">
-        <v>40</v>
       </c>
       <c r="C6">
         <f>COUNTIF(issues!$C:$C,assignees!A6)</f>
@@ -1959,10 +1959,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" t="s">
         <v>41</v>
-      </c>
-      <c r="B7" t="s">
-        <v>42</v>
       </c>
       <c r="C7">
         <f>COUNTIF(issues!$C:$C,assignees!A7)</f>
@@ -1971,10 +1971,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" t="s">
         <v>51</v>
-      </c>
-      <c r="B8" t="s">
-        <v>52</v>
       </c>
       <c r="C8">
         <f>COUNTIF(issues!$C:$C,assignees!A8)</f>
@@ -1983,10 +1983,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C9">
         <f>COUNTIF(issues!$C:$C,assignees!A9)</f>
@@ -1995,10 +1995,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" t="s">
         <v>45</v>
-      </c>
-      <c r="B10" t="s">
-        <v>46</v>
       </c>
       <c r="C10">
         <f>COUNTIF(issues!$C:$C,assignees!A10)</f>
@@ -2007,10 +2007,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" t="s">
         <v>47</v>
-      </c>
-      <c r="B11" t="s">
-        <v>48</v>
       </c>
       <c r="C11">
         <f>COUNTIF(issues!$C:$C,assignees!A11)</f>
@@ -2019,10 +2019,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" t="s">
         <v>43</v>
-      </c>
-      <c r="B12" t="s">
-        <v>44</v>
       </c>
       <c r="C12">
         <f>COUNTIF(issues!$C:$C,assignees!A12)</f>
@@ -2031,10 +2031,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" t="s">
         <v>49</v>
-      </c>
-      <c r="B13" t="s">
-        <v>50</v>
       </c>
       <c r="C13">
         <f>COUNTIF(issues!$C:$C,assignees!A13)</f>
@@ -2043,10 +2043,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" t="s">
         <v>55</v>
-      </c>
-      <c r="B14" t="s">
-        <v>56</v>
       </c>
       <c r="C14">
         <f>COUNTIF(issues!$C:$C,assignees!A14)</f>
@@ -2055,10 +2055,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" t="s">
         <v>70</v>
-      </c>
-      <c r="B15" t="s">
-        <v>71</v>
       </c>
       <c r="C15">
         <f>COUNTIF(issues!$C:$C,assignees!A15)</f>
@@ -2067,10 +2067,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B16" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C16">
         <f>COUNTIF(issues!$C:$C,assignees!A16)</f>
@@ -2079,10 +2079,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C17">
         <f>COUNTIF(issues!$C:$C,assignees!A17)</f>
@@ -2091,10 +2091,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B18" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C18">
         <f>COUNTIF(issues!$C:$C,assignees!A18)</f>
@@ -2103,10 +2103,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" t="s">
         <v>61</v>
-      </c>
-      <c r="B19" t="s">
-        <v>62</v>
       </c>
       <c r="C19">
         <f>COUNTIF(issues!$C:$C,assignees!A19)</f>
@@ -2115,10 +2115,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" t="s">
         <v>65</v>
-      </c>
-      <c r="B20" t="s">
-        <v>66</v>
       </c>
       <c r="C20">
         <f>COUNTIF(issues!$C:$C,assignees!A20)</f>
@@ -2127,10 +2127,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B21" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C21">
         <f>COUNTIF(issues!$C:$C,assignees!A21)</f>
@@ -2139,10 +2139,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" t="s">
         <v>53</v>
-      </c>
-      <c r="B22" t="s">
-        <v>54</v>
       </c>
       <c r="C22">
         <f>COUNTIF(issues!$C:$C,assignees!A22)</f>
@@ -2151,10 +2151,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" t="s">
         <v>57</v>
-      </c>
-      <c r="B23" t="s">
-        <v>58</v>
       </c>
       <c r="C23">
         <f>COUNTIF(issues!$C:$C,assignees!A23)</f>
@@ -2163,10 +2163,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" t="s">
         <v>59</v>
-      </c>
-      <c r="B24" t="s">
-        <v>60</v>
       </c>
       <c r="C24">
         <f>COUNTIF(issues!$C:$C,assignees!A24)</f>
@@ -2175,10 +2175,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" t="s">
         <v>63</v>
-      </c>
-      <c r="B25" t="s">
-        <v>64</v>
       </c>
       <c r="C25">
         <f>COUNTIF(issues!$C:$C,assignees!A25)</f>
@@ -2187,10 +2187,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" t="s">
         <v>67</v>
-      </c>
-      <c r="B26" t="s">
-        <v>68</v>
       </c>
       <c r="C26">
         <f>COUNTIF(issues!$C:$C,assignees!A26)</f>
@@ -2199,10 +2199,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B27" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C27">
         <f>COUNTIF(issues!$C:$C,assignees!A27)</f>
@@ -2211,10 +2211,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B28" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C28">
         <f>COUNTIF(issues!$C:$C,assignees!A28)</f>
@@ -2223,10 +2223,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C29">
         <f>COUNTIF(issues!$C:$C,assignees!A29)</f>
@@ -2235,10 +2235,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B30" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C30">
         <f>COUNTIF(issues!$C:$C,assignees!A30)</f>
@@ -2247,10 +2247,10 @@
     </row>
     <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C31">
         <f>COUNTIF(issues!$C:$C,assignees!A31)</f>
@@ -2259,10 +2259,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B32" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C32">
         <f>COUNTIF(issues!$C:$C,assignees!A32)</f>
@@ -2271,10 +2271,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B33" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C33">
         <f>COUNTIF(issues!$C:$C,assignees!A33)</f>
@@ -2283,10 +2283,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B34" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C34">
         <f>COUNTIF(issues!$C:$C,assignees!A34)</f>
@@ -2295,10 +2295,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B35" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C35">
         <f>COUNTIF(issues!$C:$C,assignees!A35)</f>
@@ -2307,10 +2307,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B36" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C36">
         <f>COUNTIF(issues!$C:$C,assignees!A36)</f>
@@ -2319,10 +2319,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B37" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C37">
         <f>COUNTIF(issues!$C:$C,assignees!A37)</f>

</xml_diff>

<commit_message>
Update Unscripted testing list and Formatting plots images
</commit_message>
<xml_diff>
--- a/Project-Management/Tools/RoadmapUpdate/issue_template.xlsx
+++ b/Project-Management/Tools/RoadmapUpdate/issue_template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmo84564\mantid-documents\Project-Management\Tools\RoadmapUpdate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielmurphy/new/documents/Project-Management/Tools/RoadmapUpdate/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97BA7B29-8A8D-F44D-8294-F38E49624834}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34545" yWindow="-12855" windowWidth="31665" windowHeight="16500"/>
+    <workbookView xWindow="1040" yWindow="460" windowWidth="27760" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="issues" sheetId="1" r:id="rId1"/>
@@ -18,12 +19,22 @@
   <externalReferences>
     <externalReference r:id="rId3"/>
   </externalReferences>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="143">
   <si>
     <t>Title</t>
   </si>
@@ -49,18 +60,6 @@
     <t>Unscripted Testing DGSReduction</t>
   </si>
   <si>
-    <t>Unscripted Testing Mantidplot Group 4</t>
-  </si>
-  <si>
-    <t>Unscripted Testing Mantidplot Group 3</t>
-  </si>
-  <si>
-    <t>Unscripted Testing Mantidplot Group 2</t>
-  </si>
-  <si>
-    <t>Unscripted Testing Mantidplot Group 1</t>
-  </si>
-  <si>
     <t>Unscripted Testing Muon</t>
   </si>
   <si>
@@ -242,9 +241,6 @@
   </si>
   <si>
     <t>Elliot Oram</t>
-  </si>
-  <si>
-    <t>See https://www.mantidproject.org/Unscripted_Manual_Testing#Groups</t>
   </si>
   <si>
     <t>Unscripted Testing TOFConverter</t>
@@ -262,10 +258,6 @@
   </si>
   <si>
     <t>http://developer.mantidproject.org/Testing/ErrorReporter-ProjectRecovery/ErrorReporterTesting.html</t>
-  </si>
-  <si>
-    <t>See instructions at http://docs.mantidproject.org/v3.9.0/interfaces/Muon_Analysis_unscripted_testing_guide.html
-http://developer.mantidproject.org/Testing/MuonInterface/MuonTesting.html</t>
   </si>
   <si>
     <t>Follow:  http://www.mantidproject.org/Direct:DgsReduction
@@ -431,9 +423,6 @@
     <t>Harry Saunders</t>
   </si>
   <si>
-    <t>Unscripted Testing workbench</t>
-  </si>
-  <si>
     <t>No Assigned</t>
   </si>
   <si>
@@ -528,13 +517,38 @@
   </si>
   <si>
     <t>For testing procedures see http://developer.mantidproject.org/Testing/ReflectometryGUI/ReflectometryGUITests.html</t>
+  </si>
+  <si>
+    <t>Unscripted Testing Mantidplot A</t>
+  </si>
+  <si>
+    <t>Unscripted Testing Mantidplot B</t>
+  </si>
+  <si>
+    <t>Unscripted Testing Workbench Group 2</t>
+  </si>
+  <si>
+    <t>Unscripted Testing Workbench Group 3</t>
+  </si>
+  <si>
+    <t>Unscripted Testing Workbench Group 4</t>
+  </si>
+  <si>
+    <t>Unscripted Testing Workbench Group 1</t>
+  </si>
+  <si>
+    <t>http://developer.mantidproject.org/Testing/Core/Core.html</t>
+  </si>
+  <si>
+    <t>See instructions at https://developer.mantidproject.org/Testing/MuonAnalysis_test_guides/index.html
+http://developer.mantidproject.org/Testing/MuonInterface/MuonTesting.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="21" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1034,7 +1048,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1055,6 +1069,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1203,6 +1218,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1238,6 +1270,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1413,22 +1462,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A27" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="46" style="1" customWidth="1"/>
-    <col min="2" max="2" width="72.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="72.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="16">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1439,432 +1488,444 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="64">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C2" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="16">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="112">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C5" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="32">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16">
+      <c r="A7" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="17">
+      <c r="A8" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="16">
+      <c r="A9" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="16">
+      <c r="A10" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="C10" s="7"/>
+    </row>
+    <row r="11" spans="1:5" ht="16">
+      <c r="A11" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B11" s="1" t="str">
+        <f>B9</f>
+        <v>http://developer.mantidproject.org/Testing/Core/Core.html</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="16">
+      <c r="A12" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B12" s="1" t="str">
+        <f>B11</f>
+        <v>http://developer.mantidproject.org/Testing/Core/Core.html</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="48">
+      <c r="A13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C7" s="6" t="s">
+    </row>
+    <row r="14" spans="1:5" ht="48">
+      <c r="A14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="16">
+      <c r="A15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="16">
+      <c r="A16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="16">
+      <c r="A18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="16">
+      <c r="A19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="16">
+      <c r="A20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="16">
+      <c r="A21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="409.6">
+      <c r="A22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="48">
+      <c r="A23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="16">
+      <c r="A24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="48">
+      <c r="A25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" t="s">
+        <v>119</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="16">
+      <c r="A26" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="48">
+      <c r="A27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="32">
+      <c r="A28" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C28" t="s">
+        <v>106</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="16">
+      <c r="A29" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C29" t="s">
+        <v>42</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="64">
+      <c r="A30" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C30" t="s">
+        <v>30</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="96">
+      <c r="A31" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="32">
+      <c r="A32" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C32" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="32">
+      <c r="A33" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="32">
+      <c r="A34" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="1" t="str">
-        <f>B8</f>
-        <v>See https://www.mantidproject.org/Unscripted_Manual_Testing#Groups</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="1" t="str">
-        <f>B9</f>
-        <v>See https://www.mantidproject.org/Unscripted_Manual_Testing#Groups</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="1" t="str">
-        <f>B10</f>
-        <v>See https://www.mantidproject.org/Unscripted_Manual_Testing#Groups</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C14" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C24" t="s">
-        <v>126</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C27" t="s">
-        <v>113</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C28" t="s">
-        <v>46</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C29" t="s">
-        <v>34</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C31" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>103</v>
+      <c r="B34" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:F7"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:F7" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="http://developer.mantidproject.org/Testing/IndirectInelastic/IndirectInelasticAcceptanceTests.html_x000a_"/>
+    <hyperlink ref="B2" r:id="rId1" display="http://developer.mantidproject.org/Testing/IndirectInelastic/IndirectInelasticAcceptanceTests.html_x000a_" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B10" r:id="rId2" xr:uid="{3565858B-396F-454D-84DD-1753887A47C3}"/>
+    <hyperlink ref="B8" r:id="rId3" xr:uid="{A3A08BA5-2B34-A241-890F-4CF7E72A9202}"/>
+    <hyperlink ref="B9" r:id="rId4" xr:uid="{1E29E40A-F52D-404E-A7FD-390C6069887B}"/>
+    <hyperlink ref="B7" r:id="rId5" xr:uid="{ECAECBDB-A928-1847-94C0-684975E5B596}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>[issue_templateupdate.xlsx]assignees!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>C34:C40</xm:sqref>
+          <xm:sqref>C35:C41</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
             <xm:f>assignees!$A$2:$A$37</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C33</xm:sqref>
+          <xm:sqref>C2:C34</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1873,456 +1934,456 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C32" sqref="C32:C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C2">
         <f>COUNTIF(issues!$C:$C,assignees!A2)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C3">
         <f>COUNTIF(issues!$C:$C,assignees!A3)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C4">
         <f>COUNTIF(issues!$C:$C,assignees!A4)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C5">
         <f>COUNTIF(issues!$C:$C,assignees!A5)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C6">
         <f>COUNTIF(issues!$C:$C,assignees!A6)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C7">
         <f>COUNTIF(issues!$C:$C,assignees!A7)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C8">
         <f>COUNTIF(issues!$C:$C,assignees!A8)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B9" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C9">
         <f>COUNTIF(issues!$C:$C,assignees!A9)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C10">
         <f>COUNTIF(issues!$C:$C,assignees!A10)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C11">
         <f>COUNTIF(issues!$C:$C,assignees!A11)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C12">
         <f>COUNTIF(issues!$C:$C,assignees!A12)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C13">
         <f>COUNTIF(issues!$C:$C,assignees!A13)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C14">
         <f>COUNTIF(issues!$C:$C,assignees!A14)</f>
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B15" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C15">
         <f>COUNTIF(issues!$C:$C,assignees!A15)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B16" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C16">
         <f>COUNTIF(issues!$C:$C,assignees!A16)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B17" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C17">
         <f>COUNTIF(issues!$C:$C,assignees!A17)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B18" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C18">
         <f>COUNTIF(issues!$C:$C,assignees!A18)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C19">
         <f>COUNTIF(issues!$C:$C,assignees!A19)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B20" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C20">
         <f>COUNTIF(issues!$C:$C,assignees!A20)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B21" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C21">
         <f>COUNTIF(issues!$C:$C,assignees!A21)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B22" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C22">
         <f>COUNTIF(issues!$C:$C,assignees!A22)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B23" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C23">
         <f>COUNTIF(issues!$C:$C,assignees!A23)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B24" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C24">
         <f>COUNTIF(issues!$C:$C,assignees!A24)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B25" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C25">
         <f>COUNTIF(issues!$C:$C,assignees!A25)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B26" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C26">
         <f>COUNTIF(issues!$C:$C,assignees!A26)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B27" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C27">
         <f>COUNTIF(issues!$C:$C,assignees!A27)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B28" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C28">
         <f>COUNTIF(issues!$C:$C,assignees!A28)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3">
       <c r="A29" s="6" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="C29">
         <f>COUNTIF(issues!$C:$C,assignees!A29)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B30" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C30">
         <f>COUNTIF(issues!$C:$C,assignees!A30)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="16">
       <c r="A31" s="7" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C31">
         <f>COUNTIF(issues!$C:$C,assignees!A31)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B32" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C32">
         <f>COUNTIF(issues!$C:$C,assignees!A32)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B33" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C33">
         <f>COUNTIF(issues!$C:$C,assignees!A33)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
+        <v>118</v>
+      </c>
+      <c r="B34" t="s">
         <v>125</v>
-      </c>
-      <c r="B34" t="s">
-        <v>132</v>
       </c>
       <c r="C34">
         <f>COUNTIF(issues!$C:$C,assignees!A34)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B35" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="C35">
         <f>COUNTIF(issues!$C:$C,assignees!A35)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="B36" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="C36">
         <f>COUNTIF(issues!$C:$C,assignees!A36)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B37" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C37">
         <f>COUNTIF(issues!$C:$C,assignees!A37)</f>
@@ -2330,7 +2391,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:C32">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C32">
     <sortCondition descending="1" ref="C2:C38"/>
   </sortState>
   <conditionalFormatting sqref="C1:C1048576">

</xml_diff>

<commit_message>
Update Assignees and Milestone for Unscripted Testing
</commit_message>
<xml_diff>
--- a/Project-Management/Tools/RoadmapUpdate/issue_template.xlsx
+++ b/Project-Management/Tools/RoadmapUpdate/issue_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielmurphy/new/documents/Project-Management/Tools/RoadmapUpdate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97BA7B29-8A8D-F44D-8294-F38E49624834}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BDA7EB4-2FC6-744E-BF0A-D9784D8D334D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="460" windowWidth="27760" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1040" yWindow="460" windowWidth="27760" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="issues" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="133">
   <si>
     <t>Title</t>
   </si>
@@ -114,9 +114,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>None</t>
-  </si>
-  <si>
     <t>AndreiSavici</t>
   </si>
   <si>
@@ -132,12 +129,6 @@
     <t>Gemma Guest</t>
   </si>
   <si>
-    <t>granrothge</t>
-  </si>
-  <si>
-    <t>Garrett Granroth</t>
-  </si>
-  <si>
     <t>gvardany</t>
   </si>
   <si>
@@ -156,12 +147,6 @@
     <t>Jose Borreguero</t>
   </si>
   <si>
-    <t>mantid-roman</t>
-  </si>
-  <si>
-    <t>Roman Tolchenov</t>
-  </si>
-  <si>
     <t>martyngigg</t>
   </si>
   <si>
@@ -174,12 +159,6 @@
     <t>Mathieu Doucet</t>
   </si>
   <si>
-    <t>NickDraper</t>
-  </si>
-  <si>
-    <t>Nick Draper</t>
-  </si>
-  <si>
     <t>OwenArnold</t>
   </si>
   <si>
@@ -229,18 +208,6 @@
   </si>
   <si>
     <t>Login</t>
-  </si>
-  <si>
-    <t>Mantid-Matthew</t>
-  </si>
-  <si>
-    <t>Matthew Andrew</t>
-  </si>
-  <si>
-    <t>ElliotAOram</t>
-  </si>
-  <si>
-    <t>Elliot Oram</t>
   </si>
   <si>
     <t>Unscripted Testing TOFConverter</t>
@@ -264,9 +231,6 @@
      and http://www.mantidproject.org/Create_MD_Workspace_GUI#Direct_Inelastic_Mod_Q</t>
   </si>
   <si>
-    <t>Follow: http://www.mantidproject.org/SANS_Data_Analysis_at_ISIS</t>
-  </si>
-  <si>
     <t>Follow: https://www.mantidproject.org/Fitting_QENS_I(Q,_t)</t>
   </si>
   <si>
@@ -292,10 +256,6 @@
   </si>
   <si>
     <t>Follow: http://docs.mantidproject.org/nightly/interfaces/Engineering%20Diffraction%20Test%20Guide.html</t>
-  </si>
-  <si>
-    <t>* Follow the examples at http://docs.mantidproject.org/nightly/concepts/WorkspaceGroup.html 
-* Ensure MantidPlot displays Group Workspaces correctly in the workspace tree</t>
   </si>
   <si>
     <t>Make sure that inputs and outputs work sensibly, stress test with some bad inputs (e.g. letters in a numeric input)
@@ -411,49 +371,13 @@
     <t>?</t>
   </si>
   <si>
-    <t>alicerussell1</t>
-  </si>
-  <si>
-    <t>Alice Russell</t>
-  </si>
-  <si>
-    <t>hsautessella</t>
-  </si>
-  <si>
-    <t>Harry Saunders</t>
-  </si>
-  <si>
     <t>No Assigned</t>
   </si>
   <si>
-    <t>PhilColebrooke</t>
-  </si>
-  <si>
-    <t>Philip Colebrooke</t>
-  </si>
-  <si>
-    <t>giovannidisiena</t>
-  </si>
-  <si>
-    <t>Giovanni Di Siena</t>
-  </si>
-  <si>
-    <t>ConorMFinn</t>
-  </si>
-  <si>
-    <t>Conor Finn</t>
-  </si>
-  <si>
     <t>Harrietbrown</t>
   </si>
   <si>
     <t>Harriet Brown</t>
-  </si>
-  <si>
-    <t>ciaranightingale</t>
-  </si>
-  <si>
-    <t>Ciara Nightingale</t>
   </si>
   <si>
     <t>See https://mantidproject.github.io/mslice/ and follow Quick Start, this should probably be tested in iDAaaS</t>
@@ -542,6 +466,52 @@
   <si>
     <t>See instructions at https://developer.mantidproject.org/Testing/MuonAnalysis_test_guides/index.html
 http://developer.mantidproject.org/Testing/MuonInterface/MuonTesting.html</t>
+  </si>
+  <si>
+    <t>Anthony Lim</t>
+  </si>
+  <si>
+    <t>clayton-tom</t>
+  </si>
+  <si>
+    <t>Tom Clayton</t>
+  </si>
+  <si>
+    <t>rprospero</t>
+  </si>
+  <si>
+    <t>Adam Washington</t>
+  </si>
+  <si>
+    <t>tolu28-coder</t>
+  </si>
+  <si>
+    <t>Matt-Cumber</t>
+  </si>
+  <si>
+    <t>Matthew Cumber</t>
+  </si>
+  <si>
+    <t>Toluwalase Agoro</t>
+  </si>
+  <si>
+    <t>joseph-torsney</t>
+  </si>
+  <si>
+    <t>Joseph Torsney</t>
+  </si>
+  <si>
+    <t>Sections 3+4 here: https://www.mantidproject.org/Unscripted_Manual_Testing#Groups</t>
+  </si>
+  <si>
+    <t>Sections 1+2 here: https://www.mantidproject.org/Unscripted_Manual_Testing#Groups</t>
+  </si>
+  <si>
+    <t>* Follow the examples at http://docs.mantidproject.org/nightly/concepts/WorkspaceGroup.html 
+* Ensure MantidWorkbench displays Group Workspaces correctly in the workspace tree</t>
+  </si>
+  <si>
+    <t>David, is this the old interface in MantidPlot, so maybe doesn't need testing? I've assigned to you so you can decide! Follow: http://www.mantidproject.org/SANS_Data_Analysis_at_ISIS</t>
   </si>
 </sst>
 </file>
@@ -1465,8 +1435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
@@ -1488,7 +1458,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="64">
@@ -1496,13 +1466,13 @@
         <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C2" t="s">
-        <v>108</v>
+        <v>80</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16">
@@ -1510,7 +1480,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="16">
@@ -1518,7 +1488,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="112">
@@ -1526,13 +1496,13 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="32">
@@ -1540,91 +1510,91 @@
         <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16">
       <c r="A7" s="1" t="s">
-        <v>140</v>
+        <v>115</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>141</v>
+        <v>116</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="17">
       <c r="A8" s="1" t="s">
-        <v>137</v>
+        <v>112</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>141</v>
+        <v>116</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16">
       <c r="A9" s="1" t="s">
-        <v>138</v>
+        <v>113</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>141</v>
+        <v>116</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="16">
       <c r="A10" s="1" t="s">
-        <v>139</v>
+        <v>114</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="C10" s="7"/>
+        <v>116</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="16">
       <c r="A11" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B11" s="1" t="str">
-        <f>B9</f>
-        <v>http://developer.mantidproject.org/Testing/Core/Core.html</v>
+        <v>111</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>129</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="16">
       <c r="A12" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B12" s="1" t="str">
-        <f>B11</f>
-        <v>http://developer.mantidproject.org/Testing/Core/Core.html</v>
+        <v>110</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>130</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="48">
@@ -1632,41 +1602,41 @@
         <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>142</v>
+        <v>117</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="48">
       <c r="A14" s="1" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>99</v>
+        <v>123</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="16">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="32">
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>74</v>
+        <v>132</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>94</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="16">
@@ -1674,7 +1644,7 @@
         <v>10</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="12.75" customHeight="1">
@@ -1682,7 +1652,7 @@
         <v>11</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="16">
@@ -1690,7 +1660,7 @@
         <v>12</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="16">
@@ -1698,13 +1668,13 @@
         <v>13</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="16">
@@ -1712,7 +1682,7 @@
         <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>46</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="16">
@@ -1720,7 +1690,7 @@
         <v>15</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="409.6">
@@ -1728,10 +1698,10 @@
         <v>16</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="48">
@@ -1739,13 +1709,13 @@
         <v>17</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="16">
@@ -1756,7 +1726,7 @@
         <v>19</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="48">
@@ -1764,13 +1734,13 @@
         <v>20</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>84</v>
+        <v>131</v>
       </c>
       <c r="C25" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="16">
@@ -1781,7 +1751,7 @@
         <v>22</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="48">
@@ -1789,44 +1759,44 @@
         <v>23</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>46</v>
+        <v>127</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="32">
       <c r="A28" s="1" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>134</v>
+        <v>109</v>
       </c>
       <c r="C28" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="16">
       <c r="A29" s="1" t="s">
-        <v>129</v>
+        <v>104</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="C29" t="s">
-        <v>42</v>
+        <v>87</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="64">
@@ -1834,69 +1804,69 @@
         <v>24</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>131</v>
+        <v>106</v>
       </c>
       <c r="C30" t="s">
-        <v>30</v>
+        <v>121</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>132</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="96">
       <c r="A31" s="1" t="s">
-        <v>123</v>
+        <v>98</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>112</v>
+        <v>90</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="32">
       <c r="A32" s="1" t="s">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
       <c r="C32" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="32">
       <c r="A33" s="1" t="s">
-        <v>121</v>
+        <v>96</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>119</v>
+        <v>29</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="32">
       <c r="A34" s="1" t="s">
-        <v>122</v>
+        <v>97</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>65</v>
+        <v>124</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1923,7 +1893,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
-            <xm:f>assignees!$A$2:$A$37</xm:f>
+            <xm:f>assignees!$A$4:$A$21</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C34</xm:sqref>
         </x14:dataValidation>
@@ -1935,10 +1905,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32:C37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1949,21 +1919,21 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="C2">
         <f>COUNTIF(issues!$C:$C,assignees!A2)</f>
@@ -1972,106 +1942,106 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>79</v>
       </c>
       <c r="C3">
         <f>COUNTIF(issues!$C:$C,assignees!A3)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>118</v>
       </c>
       <c r="C4">
         <f>COUNTIF(issues!$C:$C,assignees!A4)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C5">
         <f>COUNTIF(issues!$C:$C,assignees!A5)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>87</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>88</v>
       </c>
       <c r="C6">
         <f>COUNTIF(issues!$C:$C,assignees!A6)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C7">
         <f>COUNTIF(issues!$C:$C,assignees!A7)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C8">
         <f>COUNTIF(issues!$C:$C,assignees!A8)</f>
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>110</v>
+        <v>49</v>
       </c>
       <c r="B9" t="s">
-        <v>111</v>
+        <v>50</v>
       </c>
       <c r="C9">
         <f>COUNTIF(issues!$C:$C,assignees!A9)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="C10">
         <f>COUNTIF(issues!$C:$C,assignees!A10)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>127</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>128</v>
       </c>
       <c r="C11">
         <f>COUNTIF(issues!$C:$C,assignees!A11)</f>
@@ -2080,46 +2050,46 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>81</v>
       </c>
       <c r="C12">
         <f>COUNTIF(issues!$C:$C,assignees!A12)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" t="s">
-        <v>45</v>
+      <c r="A13" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>125</v>
       </c>
       <c r="C13">
         <f>COUNTIF(issues!$C:$C,assignees!A13)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>123</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>126</v>
       </c>
       <c r="C14">
         <f>COUNTIF(issues!$C:$C,assignees!A14)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
-        <v>65</v>
-      </c>
-      <c r="B15" t="s">
-        <v>66</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="16">
+      <c r="A15" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>122</v>
       </c>
       <c r="C15">
         <f>COUNTIF(issues!$C:$C,assignees!A15)</f>
@@ -2128,82 +2098,82 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>89</v>
+        <v>119</v>
       </c>
       <c r="B16" t="s">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="C16">
         <f>COUNTIF(issues!$C:$C,assignees!A16)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B17" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C17">
         <f>COUNTIF(issues!$C:$C,assignees!A17)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B18" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C18">
         <f>COUNTIF(issues!$C:$C,assignees!A18)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>56</v>
+        <v>90</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>101</v>
       </c>
       <c r="C19">
         <f>COUNTIF(issues!$C:$C,assignees!A19)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>92</v>
       </c>
       <c r="B20" t="s">
-        <v>61</v>
+        <v>102</v>
       </c>
       <c r="C20">
         <f>COUNTIF(issues!$C:$C,assignees!A20)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B21" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C21">
         <f>COUNTIF(issues!$C:$C,assignees!A21)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C22">
         <f>COUNTIF(issues!$C:$C,assignees!A22)</f>
@@ -2212,10 +2182,10 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="C23">
         <f>COUNTIF(issues!$C:$C,assignees!A23)</f>
@@ -2224,10 +2194,10 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="C24">
         <f>COUNTIF(issues!$C:$C,assignees!A24)</f>
@@ -2236,10 +2206,10 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="B25" t="s">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="C25">
         <f>COUNTIF(issues!$C:$C,assignees!A25)</f>
@@ -2248,10 +2218,10 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>62</v>
+        <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="C26">
         <f>COUNTIF(issues!$C:$C,assignees!A26)</f>
@@ -2260,10 +2230,10 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="B27" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="C27">
         <f>COUNTIF(issues!$C:$C,assignees!A27)</f>
@@ -2272,10 +2242,10 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>93</v>
+        <v>45</v>
       </c>
       <c r="B28" t="s">
-        <v>94</v>
+        <v>46</v>
       </c>
       <c r="C28">
         <f>COUNTIF(issues!$C:$C,assignees!A28)</f>
@@ -2283,116 +2253,44 @@
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>105</v>
+      <c r="A29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" t="s">
+        <v>48</v>
       </c>
       <c r="C29">
         <f>COUNTIF(issues!$C:$C,assignees!A29)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>106</v>
+        <v>51</v>
       </c>
       <c r="B30" t="s">
-        <v>107</v>
+        <v>52</v>
       </c>
       <c r="C30">
         <f>COUNTIF(issues!$C:$C,assignees!A30)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="16">
-      <c r="A31" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>109</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" t="s">
+        <v>56</v>
       </c>
       <c r="C31">
         <f>COUNTIF(issues!$C:$C,assignees!A31)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" t="s">
-        <v>112</v>
-      </c>
-      <c r="B32" t="s">
-        <v>113</v>
-      </c>
-      <c r="C32">
-        <f>COUNTIF(issues!$C:$C,assignees!A32)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" t="s">
-        <v>119</v>
-      </c>
-      <c r="B33" t="s">
-        <v>120</v>
-      </c>
-      <c r="C33">
-        <f>COUNTIF(issues!$C:$C,assignees!A33)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" t="s">
-        <v>118</v>
-      </c>
-      <c r="B34" t="s">
-        <v>125</v>
-      </c>
-      <c r="C34">
-        <f>COUNTIF(issues!$C:$C,assignees!A34)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
-        <v>115</v>
-      </c>
-      <c r="B35" t="s">
-        <v>126</v>
-      </c>
-      <c r="C35">
-        <f>COUNTIF(issues!$C:$C,assignees!A35)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" t="s">
-        <v>117</v>
-      </c>
-      <c r="B36" t="s">
-        <v>127</v>
-      </c>
-      <c r="C36">
-        <f>COUNTIF(issues!$C:$C,assignees!A36)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" t="s">
-        <v>116</v>
-      </c>
-      <c r="B37" t="s">
-        <v>128</v>
-      </c>
-      <c r="C37">
-        <f>COUNTIF(issues!$C:$C,assignees!A37)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C32">
-    <sortCondition descending="1" ref="C2:C38"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:C16">
+    <sortCondition descending="1" ref="C4:C27"/>
   </sortState>
   <conditionalFormatting sqref="C1:C1048576">
     <cfRule type="colorScale" priority="1">

</xml_diff>

<commit_message>
Refs #0. Update manual testing documents.
</commit_message>
<xml_diff>
--- a/Project-Management/Tools/RoadmapUpdate/issue_template.xlsx
+++ b/Project-Management/Tools/RoadmapUpdate/issue_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\documents\Project-Management\Tools\RoadmapUpdate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlc47243\Documents\mantid-development\mantid-docs\documents\Project-Management\Tools\RoadmapUpdate\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -243,9 +243,6 @@
     <t>small</t>
   </si>
   <si>
-    <t>Follow: http://docs.mantidproject.org/nightly/interfaces/Engineering%20Diffraction%20Test%20Guide.html</t>
-  </si>
-  <si>
     <t>Make sure that inputs and outputs work sensibly, stress test with some bad inputs (e.g. letters in a numeric input)
 See http://docs.mantidproject.org/v3.7.2/interfaces/SampleTransmissionCalculator.html</t>
   </si>
@@ -447,6 +444,9 @@
 [ ] 9. Play around with window - resizing, adjusting peak table size
 [ ] 10. Saving plot
 [ ] 11. Delete/rename underlying workspaces (at present sliceviewer does not update)</t>
+  </si>
+  <si>
+    <t>Follow: https://developer.mantidproject.org/Testing/EngineeringDiffraction/EngineeringDiffractionTestGuide.html</t>
   </si>
 </sst>
 </file>
@@ -1336,8 +1336,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:B32"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1367,10 +1367,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>63</v>
@@ -1397,10 +1397,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>64</v>
@@ -1414,18 +1414,18 @@
         <v>60</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>111</v>
-      </c>
       <c r="C7" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>63</v>
@@ -1433,13 +1433,13 @@
     </row>
     <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>63</v>
@@ -1447,13 +1447,13 @@
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>63</v>
@@ -1461,13 +1461,13 @@
     </row>
     <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -1475,7 +1475,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>27</v>
@@ -1489,10 +1489,10 @@
         <v>57</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>66</v>
@@ -1503,10 +1503,10 @@
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>67</v>
@@ -1544,7 +1544,7 @@
         <v>61</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>68</v>
@@ -1555,7 +1555,7 @@
         <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1571,10 +1571,10 @@
         <v>16</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>69</v>
+        <v>128</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>67</v>
@@ -1596,10 +1596,10 @@
         <v>19</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>68</v>
@@ -1621,10 +1621,10 @@
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>66</v>
@@ -1632,16 +1632,16 @@
     </row>
     <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="C25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>65</v>
@@ -1649,16 +1649,16 @@
     </row>
     <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="C26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -1666,46 +1666,46 @@
         <v>23</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C27" t="s">
+        <v>115</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="C27" t="s">
-        <v>116</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C29" t="s">
         <v>86</v>
-      </c>
-      <c r="C29" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>58</v>
@@ -1714,29 +1714,29 @@
         <v>28</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="285" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1795,15 +1795,15 @@
         <v>24</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" t="s">
         <v>74</v>
-      </c>
-      <c r="B2" t="s">
-        <v>75</v>
       </c>
       <c r="C2">
         <f>COUNTIF(issues!$C:$C,assignees!A2)</f>
@@ -1812,10 +1812,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" t="s">
         <v>76</v>
-      </c>
-      <c r="B3" t="s">
-        <v>77</v>
       </c>
       <c r="C3">
         <f>COUNTIF(issues!$C:$C,assignees!A3)</f>
@@ -1827,7 +1827,7 @@
         <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C4">
         <f>COUNTIF(issues!$C:$C,assignees!A4)</f>
@@ -1848,10 +1848,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" t="s">
         <v>84</v>
-      </c>
-      <c r="B6" t="s">
-        <v>85</v>
       </c>
       <c r="C6">
         <f>COUNTIF(issues!$C:$C,assignees!A6)</f>
@@ -1908,10 +1908,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>121</v>
+      </c>
+      <c r="B11" t="s">
         <v>122</v>
-      </c>
-      <c r="B11" t="s">
-        <v>123</v>
       </c>
       <c r="C11">
         <f>COUNTIF(issues!$C:$C,assignees!A11)</f>
@@ -1920,10 +1920,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" t="s">
         <v>78</v>
-      </c>
-      <c r="B12" t="s">
-        <v>79</v>
       </c>
       <c r="C12">
         <f>COUNTIF(issues!$C:$C,assignees!A12)</f>
@@ -1932,10 +1932,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>119</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>120</v>
       </c>
       <c r="C13">
         <f>COUNTIF(issues!$C:$C,assignees!A13)</f>
@@ -1944,10 +1944,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C14">
         <f>COUNTIF(issues!$C:$C,assignees!A14)</f>
@@ -1956,10 +1956,10 @@
     </row>
     <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>116</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>117</v>
       </c>
       <c r="C15">
         <f>COUNTIF(issues!$C:$C,assignees!A15)</f>
@@ -1968,10 +1968,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>113</v>
+      </c>
+      <c r="B16" t="s">
         <v>114</v>
-      </c>
-      <c r="B16" t="s">
-        <v>115</v>
       </c>
       <c r="C16">
         <f>COUNTIF(issues!$C:$C,assignees!A16)</f>
@@ -1980,10 +1980,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" t="s">
         <v>91</v>
-      </c>
-      <c r="B17" t="s">
-        <v>92</v>
       </c>
       <c r="C17">
         <f>COUNTIF(issues!$C:$C,assignees!A17)</f>
@@ -1992,10 +1992,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C18">
         <f>COUNTIF(issues!$C:$C,assignees!A18)</f>
@@ -2004,10 +2004,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C19">
         <f>COUNTIF(issues!$C:$C,assignees!A19)</f>
@@ -2016,10 +2016,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C20">
         <f>COUNTIF(issues!$C:$C,assignees!A20)</f>
@@ -2028,10 +2028,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C21">
         <f>COUNTIF(issues!$C:$C,assignees!A21)</f>

</xml_diff>

<commit_message>
Refs #0. Update manual testing excel sheets.
</commit_message>
<xml_diff>
--- a/Project-Management/Tools/RoadmapUpdate/issue_template.xlsx
+++ b/Project-Management/Tools/RoadmapUpdate/issue_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1035" yWindow="465" windowWidth="27765" windowHeight="17535"/>
+    <workbookView xWindow="1033" yWindow="467" windowWidth="27767" windowHeight="17533"/>
   </bookViews>
   <sheets>
     <sheet name="issues" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="127">
   <si>
     <t>Title</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>Unscripted Testing ORNL SANS</t>
-  </si>
-  <si>
-    <t>Unscripted Testing Multi dataset fitting</t>
   </si>
   <si>
     <t>Unscripted Testing FilterEvents</t>
@@ -219,9 +216,6 @@
      and http://www.mantidproject.org/Create_MD_Workspace_GUI#Direct_Inelastic_Mod_Q</t>
   </si>
   <si>
-    <t>Follow: https://www.mantidproject.org/Fitting_QENS_I(Q,_t)</t>
-  </si>
-  <si>
     <t>size</t>
   </si>
   <si>
@@ -249,12 +243,6 @@
   <si>
     <t>Make sure that inputs and outputs work sensibly, stress test with some bad inputs (e.g. letters in a numeric input)
 See http://docs.mantidproject.org/v3.12.0/interfaces/TOF%20Converter.html</t>
-  </si>
-  <si>
-    <t>* Build a docs-html target of Mantid
-* Check against the online documentation (http://docs.mantidproject.org/nightly/tutorials/mantid_basic_course/index.html#mantid-basic-course)
-* Open up the basic course (docs/html/tutorials/mantid_basic_course/index.html)
-* Check that the pages in there make sense</t>
   </si>
   <si>
     <t xml:space="preserve">Follow the directions at: http://developer.mantidproject.org/Testing/IndirectInelastic/IndirectInelasticAcceptanceTests.html
@@ -447,6 +435,13 @@
   </si>
   <si>
     <t>Follow: https://developer.mantidproject.org/Testing/EngineeringDiffraction/EngineeringDiffractionTestGuide.html</t>
+  </si>
+  <si>
+    <t>* Build a docs-html target of Mantid
+* Build docs-qtassistant and docs-qthelp so that autogenerated plots are available
+* Check against the online documentation (http://docs.mantidproject.org/nightly/tutorials/mantid_basic_course/index.html#mantid-basic-course)
+* Open up the basic course (docs/html/tutorials/mantid_basic_course/index.html)
+* Check that the pages in there make sense</t>
   </si>
 </sst>
 </file>
@@ -1334,21 +1329,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="46" style="1" customWidth="1"/>
-    <col min="2" max="2" width="72.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="72.703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.87890625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.1171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1359,384 +1354,370 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="57.35" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="186.35" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="43" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="16.350000000000001" x14ac:dyDescent="0.65">
+      <c r="A8" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="E9" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:5" ht="43" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="43" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="43" x14ac:dyDescent="0.5">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C13" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C18" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C18" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="43" x14ac:dyDescent="0.5">
       <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="43" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="C21" t="s">
+        <v>80</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+      <c r="A23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+      <c r="A24" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A25" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C25" t="s">
+        <v>80</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="57.35" x14ac:dyDescent="0.5">
+      <c r="A26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C26" t="s">
+        <v>112</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="100.35" x14ac:dyDescent="0.5">
+      <c r="A27" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C25" t="s">
-        <v>87</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="E27" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A28" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28" t="s">
         <v>83</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C27" t="s">
-        <v>115</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A29" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C29" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A30" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>58</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>28</v>
+        <v>115</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="229.35" x14ac:dyDescent="0.5">
       <c r="A31" s="1" t="s">
-        <v>93</v>
+        <v>123</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="285" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1754,18 +1735,24 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>[issue_templateupdate.xlsx]assignees!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>C32:C38</xm:sqref>
+          <xm:sqref>C31:C37</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>assignees!$A$4:$A$21</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C31</xm:sqref>
+          <xm:sqref>C21:C30 C2:C13 C15:C19</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>assignees!$A$4:$A$22</xm:f>
+          </x14:formula1>
+          <xm:sqref>C20 C14</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1778,380 +1765,380 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD15"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.87890625" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C2">
         <f>COUNTIF(issues!$C:$C,assignees!A2)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C3">
         <f>COUNTIF(issues!$C:$C,assignees!A3)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C4">
         <f>COUNTIF(issues!$C:$C,assignees!A4)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
         <v>28</v>
-      </c>
-      <c r="B5" t="s">
-        <v>29</v>
       </c>
       <c r="C5">
         <f>COUNTIF(issues!$C:$C,assignees!A5)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C6">
         <f>COUNTIF(issues!$C:$C,assignees!A6)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
         <v>36</v>
-      </c>
-      <c r="B7" t="s">
-        <v>37</v>
       </c>
       <c r="C7">
         <f>COUNTIF(issues!$C:$C,assignees!A7)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s">
         <v>42</v>
-      </c>
-      <c r="B8" t="s">
-        <v>43</v>
       </c>
       <c r="C8">
         <f>COUNTIF(issues!$C:$C,assignees!A8)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" t="s">
         <v>48</v>
-      </c>
-      <c r="B9" t="s">
-        <v>49</v>
       </c>
       <c r="C9">
         <f>COUNTIF(issues!$C:$C,assignees!A9)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" t="s">
         <v>52</v>
-      </c>
-      <c r="B10" t="s">
-        <v>53</v>
       </c>
       <c r="C10">
         <f>COUNTIF(issues!$C:$C,assignees!A10)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B11" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C11">
         <f>COUNTIF(issues!$C:$C,assignees!A11)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B12" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C12">
         <f>COUNTIF(issues!$C:$C,assignees!A12)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A13" s="6" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C13">
         <f>COUNTIF(issues!$C:$C,assignees!A13)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
+        <v>114</v>
+      </c>
+      <c r="B14" t="s">
         <v>117</v>
-      </c>
-      <c r="B14" t="s">
-        <v>120</v>
       </c>
       <c r="C14">
         <f>COUNTIF(issues!$C:$C,assignees!A14)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="7" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C15">
         <f>COUNTIF(issues!$C:$C,assignees!A15)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B16" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C16">
         <f>COUNTIF(issues!$C:$C,assignees!A16)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B17" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C17">
         <f>COUNTIF(issues!$C:$C,assignees!A17)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B18" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C18">
         <f>COUNTIF(issues!$C:$C,assignees!A18)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B19" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C19">
         <f>COUNTIF(issues!$C:$C,assignees!A19)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B20" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C20">
         <f>COUNTIF(issues!$C:$C,assignees!A20)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B21" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C21">
         <f>COUNTIF(issues!$C:$C,assignees!A21)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C22">
         <f>COUNTIF(issues!$C:$C,assignees!A22)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C23">
         <f>COUNTIF(issues!$C:$C,assignees!A23)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C24">
         <f>COUNTIF(issues!$C:$C,assignees!A24)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C25">
         <f>COUNTIF(issues!$C:$C,assignees!A25)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B26" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C26">
         <f>COUNTIF(issues!$C:$C,assignees!A26)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" t="s">
         <v>40</v>
-      </c>
-      <c r="B27" t="s">
-        <v>41</v>
       </c>
       <c r="C27">
         <f>COUNTIF(issues!$C:$C,assignees!A27)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" t="s">
         <v>44</v>
-      </c>
-      <c r="B28" t="s">
-        <v>45</v>
       </c>
       <c r="C28">
         <f>COUNTIF(issues!$C:$C,assignees!A28)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" t="s">
         <v>46</v>
-      </c>
-      <c r="B29" t="s">
-        <v>47</v>
       </c>
       <c r="C29">
         <f>COUNTIF(issues!$C:$C,assignees!A29)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" t="s">
         <v>50</v>
-      </c>
-      <c r="B30" t="s">
-        <v>51</v>
       </c>
       <c r="C30">
         <f>COUNTIF(issues!$C:$C,assignees!A30)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A31" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" t="s">
         <v>54</v>
-      </c>
-      <c r="B31" t="s">
-        <v>55</v>
       </c>
       <c r="C31">
         <f>COUNTIF(issues!$C:$C,assignees!A31)</f>

</xml_diff>